<commit_message>
update from richard nov 23
</commit_message>
<xml_diff>
--- a/data/historical/source/wages_historical.xlsx
+++ b/data/historical/source/wages_historical.xlsx
@@ -9,15 +9,15 @@
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+  <si>
+    <t>Real Average Weekly Wages; Year/Year: January 2008 -- October 2015</t>
+  </si>
   <si>
     <t>Source: Bureau of Labor Statistics</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Wyoming</t>
-  </si>
-  <si>
-    <t>Real Average Weekly Wages; Year/Year: January 2008 -- September 2015</t>
   </si>
 </sst>
 </file>
@@ -2096,504 +2093,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TABLE"/>
-      <sheetName val="FRED"/>
-      <sheetName val="CPI_FRED"/>
-      <sheetName val="CPI_BLS"/>
-      <sheetName val="Key"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="8">
-          <cell r="B8">
-            <v>710.7</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>39448</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>39479</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>39508</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>39539</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>39569</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>39600</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>39630</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>39661</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>39692</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>39722</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>39753</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>39783</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>39814</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>39845</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>39873</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>39904</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>39934</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>39965</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>39995</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>40026</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>40057</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>40087</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>40118</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>40148</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>40179</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>40210</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>40238</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>40269</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>40299</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>40330</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>40360</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>40391</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>40422</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>40452</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>40483</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55">
-            <v>40513</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56">
-            <v>40544</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57">
-            <v>40575</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58">
-            <v>40603</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59">
-            <v>40634</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60">
-            <v>40664</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61">
-            <v>40695</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62">
-            <v>40725</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63">
-            <v>40756</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64">
-            <v>40787</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65">
-            <v>40817</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66">
-            <v>40848</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67">
-            <v>40878</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68">
-            <v>40909</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69">
-            <v>40940</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70">
-            <v>40969</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71">
-            <v>41000</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72">
-            <v>41030</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73">
-            <v>41061</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>41091</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75">
-            <v>41122</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76">
-            <v>41153</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77">
-            <v>41183</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78">
-            <v>41214</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79">
-            <v>41244</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80">
-            <v>41275</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81">
-            <v>41306</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>41334</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83">
-            <v>41365</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84">
-            <v>41395</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85">
-            <v>41426</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86">
-            <v>41456</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87">
-            <v>41487</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88">
-            <v>41518</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89">
-            <v>41548</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>41579</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91">
-            <v>41609</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92">
-            <v>41640</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93">
-            <v>41671</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94">
-            <v>41699</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95">
-            <v>41730</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96">
-            <v>41760</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97">
-            <v>41791</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98">
-            <v>41821</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>41852</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>41883</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>41913</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102">
-            <v>41944</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>41974</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104">
-            <v>42005</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105">
-            <v>42036</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106">
-            <v>42064</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107">
-            <v>42095</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108">
-            <v>42125</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109">
-            <v>42156</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110">
-            <v>42186</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111">
-            <v>42217</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112">
-            <v>42248</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="212">
-          <cell r="C212">
-            <v>0.85106669245452793</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2884,8 +2383,8 @@
   <dimension ref="A1:BA99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I98" sqref="I98"/>
+      <pane ySplit="5" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2909,181 +2408,180 @@
   <sheetData>
     <row r="1" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:53" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AH5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AJ5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AL5" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AN5" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AO5" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AR5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AS5" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AT5" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AU5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AV5" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AZ5" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BA5" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <f>[1]FRED!A20</f>
         <v>39448</v>
       </c>
       <c r="B6" s="6">
@@ -3245,7 +2743,6 @@
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <f>[1]FRED!A21</f>
         <v>39479</v>
       </c>
       <c r="B7" s="6">
@@ -3407,7 +2904,6 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <f>[1]FRED!A22</f>
         <v>39508</v>
       </c>
       <c r="B8" s="6">
@@ -3569,7 +3065,6 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
-        <f>[1]FRED!A23</f>
         <v>39539</v>
       </c>
       <c r="B9" s="6">
@@ -3731,7 +3226,6 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <f>[1]FRED!A24</f>
         <v>39569</v>
       </c>
       <c r="B10" s="6">
@@ -3893,7 +3387,6 @@
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
-        <f>[1]FRED!A25</f>
         <v>39600</v>
       </c>
       <c r="B11" s="6">
@@ -4055,7 +3548,6 @@
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
-        <f>[1]FRED!A26</f>
         <v>39630</v>
       </c>
       <c r="B12" s="6">
@@ -4217,7 +3709,6 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
-        <f>[1]FRED!A27</f>
         <v>39661</v>
       </c>
       <c r="B13" s="6">
@@ -4379,7 +3870,6 @@
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
-        <f>[1]FRED!A28</f>
         <v>39692</v>
       </c>
       <c r="B14" s="6">
@@ -4541,7 +4031,6 @@
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
-        <f>[1]FRED!A29</f>
         <v>39722</v>
       </c>
       <c r="B15" s="6">
@@ -4703,7 +4192,6 @@
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
-        <f>[1]FRED!A30</f>
         <v>39753</v>
       </c>
       <c r="B16" s="6">
@@ -4865,7 +4353,6 @@
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
-        <f>[1]FRED!A31</f>
         <v>39783</v>
       </c>
       <c r="B17" s="6">
@@ -5027,7 +4514,6 @@
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
-        <f>[1]FRED!A32</f>
         <v>39814</v>
       </c>
       <c r="B18" s="6">
@@ -5189,7 +4675,6 @@
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
-        <f>[1]FRED!A33</f>
         <v>39845</v>
       </c>
       <c r="B19" s="6">
@@ -5351,7 +4836,6 @@
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
-        <f>[1]FRED!A34</f>
         <v>39873</v>
       </c>
       <c r="B20" s="6">
@@ -5513,7 +4997,6 @@
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
-        <f>[1]FRED!A35</f>
         <v>39904</v>
       </c>
       <c r="B21" s="6">
@@ -5675,7 +5158,6 @@
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
-        <f>[1]FRED!A36</f>
         <v>39934</v>
       </c>
       <c r="B22" s="6">
@@ -5837,7 +5319,6 @@
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
-        <f>[1]FRED!A37</f>
         <v>39965</v>
       </c>
       <c r="B23" s="6">
@@ -5999,7 +5480,6 @@
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
-        <f>[1]FRED!A38</f>
         <v>39995</v>
       </c>
       <c r="B24" s="6">
@@ -6161,7 +5641,6 @@
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
-        <f>[1]FRED!A39</f>
         <v>40026</v>
       </c>
       <c r="B25" s="6">
@@ -6323,7 +5802,6 @@
     </row>
     <row r="26" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
-        <f>[1]FRED!A40</f>
         <v>40057</v>
       </c>
       <c r="B26" s="6">
@@ -6485,7 +5963,6 @@
     </row>
     <row r="27" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <f>[1]FRED!A41</f>
         <v>40087</v>
       </c>
       <c r="B27" s="6">
@@ -6647,7 +6124,6 @@
     </row>
     <row r="28" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
-        <f>[1]FRED!A42</f>
         <v>40118</v>
       </c>
       <c r="B28" s="6">
@@ -6809,7 +6285,6 @@
     </row>
     <row r="29" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
-        <f>[1]FRED!A43</f>
         <v>40148</v>
       </c>
       <c r="B29" s="6">
@@ -6971,7 +6446,6 @@
     </row>
     <row r="30" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
-        <f>[1]FRED!A44</f>
         <v>40179</v>
       </c>
       <c r="B30" s="6">
@@ -7133,7 +6607,6 @@
     </row>
     <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
-        <f>[1]FRED!A45</f>
         <v>40210</v>
       </c>
       <c r="B31" s="6">
@@ -7295,7 +6768,6 @@
     </row>
     <row r="32" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
-        <f>[1]FRED!A46</f>
         <v>40238</v>
       </c>
       <c r="B32" s="6">
@@ -7457,7 +6929,6 @@
     </row>
     <row r="33" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
-        <f>[1]FRED!A47</f>
         <v>40269</v>
       </c>
       <c r="B33" s="6">
@@ -7619,7 +7090,6 @@
     </row>
     <row r="34" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <f>[1]FRED!A48</f>
         <v>40299</v>
       </c>
       <c r="B34" s="6">
@@ -7781,7 +7251,6 @@
     </row>
     <row r="35" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <f>[1]FRED!A49</f>
         <v>40330</v>
       </c>
       <c r="B35" s="6">
@@ -7943,7 +7412,6 @@
     </row>
     <row r="36" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <f>[1]FRED!A50</f>
         <v>40360</v>
       </c>
       <c r="B36" s="6">
@@ -8105,7 +7573,6 @@
     </row>
     <row r="37" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
-        <f>[1]FRED!A51</f>
         <v>40391</v>
       </c>
       <c r="B37" s="6">
@@ -8267,7 +7734,6 @@
     </row>
     <row r="38" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
-        <f>[1]FRED!A52</f>
         <v>40422</v>
       </c>
       <c r="B38" s="6">
@@ -8429,7 +7895,6 @@
     </row>
     <row r="39" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
-        <f>[1]FRED!A53</f>
         <v>40452</v>
       </c>
       <c r="B39" s="6">
@@ -8591,7 +8056,6 @@
     </row>
     <row r="40" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
-        <f>[1]FRED!A54</f>
         <v>40483</v>
       </c>
       <c r="B40" s="6">
@@ -8753,7 +8217,6 @@
     </row>
     <row r="41" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
-        <f>[1]FRED!A55</f>
         <v>40513</v>
       </c>
       <c r="B41" s="6">
@@ -8915,7 +8378,6 @@
     </row>
     <row r="42" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
-        <f>[1]FRED!A56</f>
         <v>40544</v>
       </c>
       <c r="B42" s="6">
@@ -9077,7 +8539,6 @@
     </row>
     <row r="43" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
-        <f>[1]FRED!A57</f>
         <v>40575</v>
       </c>
       <c r="B43" s="6">
@@ -9239,7 +8700,6 @@
     </row>
     <row r="44" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <f>[1]FRED!A58</f>
         <v>40603</v>
       </c>
       <c r="B44" s="6">
@@ -9401,7 +8861,6 @@
     </row>
     <row r="45" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
-        <f>[1]FRED!A59</f>
         <v>40634</v>
       </c>
       <c r="B45" s="6">
@@ -9563,7 +9022,6 @@
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
-        <f>[1]FRED!A60</f>
         <v>40664</v>
       </c>
       <c r="B46" s="6">
@@ -9725,7 +9183,6 @@
     </row>
     <row r="47" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <f>[1]FRED!A61</f>
         <v>40695</v>
       </c>
       <c r="B47" s="6">
@@ -9887,7 +9344,6 @@
     </row>
     <row r="48" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
-        <f>[1]FRED!A62</f>
         <v>40725</v>
       </c>
       <c r="B48" s="6">
@@ -10049,7 +9505,6 @@
     </row>
     <row r="49" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
-        <f>[1]FRED!A63</f>
         <v>40756</v>
       </c>
       <c r="B49" s="6">
@@ -10211,7 +9666,6 @@
     </row>
     <row r="50" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
-        <f>[1]FRED!A64</f>
         <v>40787</v>
       </c>
       <c r="B50" s="6">
@@ -10373,7 +9827,6 @@
     </row>
     <row r="51" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
-        <f>[1]FRED!A65</f>
         <v>40817</v>
       </c>
       <c r="B51" s="6">
@@ -10535,7 +9988,6 @@
     </row>
     <row r="52" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
-        <f>[1]FRED!A66</f>
         <v>40848</v>
       </c>
       <c r="B52" s="6">
@@ -10697,7 +10149,6 @@
     </row>
     <row r="53" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
-        <f>[1]FRED!A67</f>
         <v>40878</v>
       </c>
       <c r="B53" s="6">
@@ -10859,7 +10310,6 @@
     </row>
     <row r="54" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
-        <f>[1]FRED!A68</f>
         <v>40909</v>
       </c>
       <c r="B54" s="6">
@@ -11021,7 +10471,6 @@
     </row>
     <row r="55" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
-        <f>[1]FRED!A69</f>
         <v>40940</v>
       </c>
       <c r="B55" s="6">
@@ -11183,7 +10632,6 @@
     </row>
     <row r="56" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
-        <f>[1]FRED!A70</f>
         <v>40969</v>
       </c>
       <c r="B56" s="6">
@@ -11345,7 +10793,6 @@
     </row>
     <row r="57" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
-        <f>[1]FRED!A71</f>
         <v>41000</v>
       </c>
       <c r="B57" s="6">
@@ -11507,7 +10954,6 @@
     </row>
     <row r="58" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
-        <f>[1]FRED!A72</f>
         <v>41030</v>
       </c>
       <c r="B58" s="6">
@@ -11669,7 +11115,6 @@
     </row>
     <row r="59" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
-        <f>[1]FRED!A73</f>
         <v>41061</v>
       </c>
       <c r="B59" s="6">
@@ -11831,7 +11276,6 @@
     </row>
     <row r="60" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
-        <f>[1]FRED!A74</f>
         <v>41091</v>
       </c>
       <c r="B60" s="6">
@@ -11993,7 +11437,6 @@
     </row>
     <row r="61" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
-        <f>[1]FRED!A75</f>
         <v>41122</v>
       </c>
       <c r="B61" s="6">
@@ -12155,7 +11598,6 @@
     </row>
     <row r="62" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
-        <f>[1]FRED!A76</f>
         <v>41153</v>
       </c>
       <c r="B62" s="6">
@@ -12317,7 +11759,6 @@
     </row>
     <row r="63" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
-        <f>[1]FRED!A77</f>
         <v>41183</v>
       </c>
       <c r="B63" s="6">
@@ -12479,7 +11920,6 @@
     </row>
     <row r="64" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
-        <f>[1]FRED!A78</f>
         <v>41214</v>
       </c>
       <c r="B64" s="6">
@@ -12641,7 +12081,6 @@
     </row>
     <row r="65" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
-        <f>[1]FRED!A79</f>
         <v>41244</v>
       </c>
       <c r="B65" s="6">
@@ -12803,7 +12242,6 @@
     </row>
     <row r="66" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
-        <f>[1]FRED!A80</f>
         <v>41275</v>
       </c>
       <c r="B66" s="6">
@@ -12965,7 +12403,6 @@
     </row>
     <row r="67" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
-        <f>[1]FRED!A81</f>
         <v>41306</v>
       </c>
       <c r="B67" s="6">
@@ -13127,7 +12564,6 @@
     </row>
     <row r="68" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
-        <f>[1]FRED!A82</f>
         <v>41334</v>
       </c>
       <c r="B68" s="6">
@@ -13289,7 +12725,6 @@
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
-        <f>[1]FRED!A83</f>
         <v>41365</v>
       </c>
       <c r="B69" s="6">
@@ -13451,7 +12886,6 @@
     </row>
     <row r="70" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
-        <f>[1]FRED!A84</f>
         <v>41395</v>
       </c>
       <c r="B70" s="6">
@@ -13613,7 +13047,6 @@
     </row>
     <row r="71" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
-        <f>[1]FRED!A85</f>
         <v>41426</v>
       </c>
       <c r="B71" s="6">
@@ -13775,7 +13208,6 @@
     </row>
     <row r="72" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
-        <f>[1]FRED!A86</f>
         <v>41456</v>
       </c>
       <c r="B72" s="6">
@@ -13937,7 +13369,6 @@
     </row>
     <row r="73" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
-        <f>[1]FRED!A87</f>
         <v>41487</v>
       </c>
       <c r="B73" s="6">
@@ -14099,7 +13530,6 @@
     </row>
     <row r="74" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
-        <f>[1]FRED!A88</f>
         <v>41518</v>
       </c>
       <c r="B74" s="6">
@@ -14261,7 +13691,6 @@
     </row>
     <row r="75" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
-        <f>[1]FRED!A89</f>
         <v>41548</v>
       </c>
       <c r="B75" s="6">
@@ -14423,7 +13852,6 @@
     </row>
     <row r="76" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
-        <f>[1]FRED!A90</f>
         <v>41579</v>
       </c>
       <c r="B76" s="6">
@@ -14585,7 +14013,6 @@
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
-        <f>[1]FRED!A91</f>
         <v>41609</v>
       </c>
       <c r="B77" s="6">
@@ -14747,7 +14174,6 @@
     </row>
     <row r="78" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
-        <f>[1]FRED!A92</f>
         <v>41640</v>
       </c>
       <c r="B78" s="6">
@@ -14909,7 +14335,6 @@
     </row>
     <row r="79" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
-        <f>[1]FRED!A93</f>
         <v>41671</v>
       </c>
       <c r="B79" s="6">
@@ -15071,7 +14496,6 @@
     </row>
     <row r="80" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
-        <f>[1]FRED!A94</f>
         <v>41699</v>
       </c>
       <c r="B80" s="6">
@@ -15233,7 +14657,6 @@
     </row>
     <row r="81" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
-        <f>[1]FRED!A95</f>
         <v>41730</v>
       </c>
       <c r="B81" s="6">
@@ -15395,7 +14818,6 @@
     </row>
     <row r="82" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
-        <f>[1]FRED!A96</f>
         <v>41760</v>
       </c>
       <c r="B82" s="6">
@@ -15557,7 +14979,6 @@
     </row>
     <row r="83" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
-        <f>[1]FRED!A97</f>
         <v>41791</v>
       </c>
       <c r="B83" s="6">
@@ -15719,7 +15140,6 @@
     </row>
     <row r="84" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
-        <f>[1]FRED!A98</f>
         <v>41821</v>
       </c>
       <c r="B84" s="6">
@@ -15881,7 +15301,6 @@
     </row>
     <row r="85" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
-        <f>[1]FRED!A99</f>
         <v>41852</v>
       </c>
       <c r="B85" s="6">
@@ -16043,7 +15462,6 @@
     </row>
     <row r="86" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
-        <f>[1]FRED!A100</f>
         <v>41883</v>
       </c>
       <c r="B86" s="6">
@@ -16205,7 +15623,6 @@
     </row>
     <row r="87" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
-        <f>[1]FRED!A101</f>
         <v>41913</v>
       </c>
       <c r="B87" s="6">
@@ -16367,7 +15784,6 @@
     </row>
     <row r="88" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
-        <f>[1]FRED!A102</f>
         <v>41944</v>
       </c>
       <c r="B88" s="6">
@@ -16529,7 +15945,6 @@
     </row>
     <row r="89" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
-        <f>[1]FRED!A103</f>
         <v>41974</v>
       </c>
       <c r="B89" s="6">
@@ -16691,7 +16106,6 @@
     </row>
     <row r="90" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
-        <f>[1]FRED!A104</f>
         <v>42005</v>
       </c>
       <c r="B90" s="6">
@@ -16853,7 +16267,6 @@
     </row>
     <row r="91" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
-        <f>[1]FRED!A105</f>
         <v>42036</v>
       </c>
       <c r="B91" s="6">
@@ -17015,7 +16428,6 @@
     </row>
     <row r="92" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
-        <f>[1]FRED!A106</f>
         <v>42064</v>
       </c>
       <c r="B92" s="6">
@@ -17177,7 +16589,6 @@
     </row>
     <row r="93" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
-        <f>[1]FRED!A107</f>
         <v>42095</v>
       </c>
       <c r="B93" s="6">
@@ -17339,7 +16750,6 @@
     </row>
     <row r="94" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
-        <f>[1]FRED!A108</f>
         <v>42125</v>
       </c>
       <c r="B94" s="6">
@@ -17501,7 +16911,6 @@
     </row>
     <row r="95" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
-        <f>[1]FRED!A109</f>
         <v>42156</v>
       </c>
       <c r="B95" s="6">
@@ -17663,7 +17072,6 @@
     </row>
     <row r="96" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
-        <f>[1]FRED!A110</f>
         <v>42186</v>
       </c>
       <c r="B96" s="6">
@@ -17825,7 +17233,6 @@
     </row>
     <row r="97" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
-        <f>[1]FRED!A111</f>
         <v>42217</v>
       </c>
       <c r="B97" s="6">
@@ -17987,169 +17394,325 @@
     </row>
     <row r="98" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
-        <f>[1]FRED!A112</f>
         <v>42248</v>
       </c>
       <c r="B98" s="6">
         <v>2.3180128372968336</v>
       </c>
       <c r="C98" s="6">
-        <v>0.29169768772211402</v>
+        <v>1.1005017013327831</v>
       </c>
       <c r="D98" s="6">
-        <v>1.3861326488171872</v>
+        <v>2.1306278272832739</v>
       </c>
       <c r="E98" s="6">
-        <v>3.5472269379134906</v>
+        <v>3.4696053285147563</v>
       </c>
       <c r="F98" s="6">
-        <v>-1.1139856721989321</v>
+        <v>-1.4526918822004753</v>
       </c>
       <c r="G98" s="6">
-        <v>2.154627555876703</v>
+        <v>1.894983351928399</v>
       </c>
       <c r="H98" s="6">
-        <v>0.97177405343942236</v>
+        <v>0.74700110289772503</v>
       </c>
       <c r="I98" s="6">
-        <v>2.8210447681350428</v>
+        <v>2.8513267917191158</v>
       </c>
       <c r="J98" s="6">
-        <v>5.6642851853694838</v>
+        <v>6.1646266236050664</v>
       </c>
       <c r="K98" s="6">
-        <v>-5.7353672129554178</v>
+        <v>-5.684904347437711</v>
       </c>
       <c r="L98" s="6">
-        <v>1.5705159733394929</v>
+        <v>1.4497611988441521</v>
       </c>
       <c r="M98" s="6">
-        <v>0.13670356104796594</v>
+        <v>-3.1705414087965629E-2</v>
       </c>
       <c r="N98" s="6">
-        <v>-3.9012848224108656</v>
+        <v>-3.4426260724629052</v>
       </c>
       <c r="O98" s="6">
-        <v>1.9801953510721324</v>
+        <v>1.673531816142465</v>
       </c>
       <c r="P98" s="6">
-        <v>2.6743982607165488</v>
+        <v>1.6667312468045905</v>
       </c>
       <c r="Q98" s="6">
-        <v>0.33673523929430876</v>
+        <v>0.71629687102618744</v>
       </c>
       <c r="R98" s="6">
-        <v>3.6494005929051645</v>
+        <v>3.1267199055027248</v>
       </c>
       <c r="S98" s="6">
-        <v>-9.0127651450361154E-2</v>
+        <v>7.1290253060657491E-2</v>
       </c>
       <c r="T98" s="6">
-        <v>4.4653312051113812</v>
+        <v>4.563695160672947</v>
       </c>
       <c r="U98" s="6">
-        <v>-1.7324064088952782</v>
+        <v>-1.9086364013446206</v>
       </c>
       <c r="V98" s="6">
-        <v>3.1770443426877786</v>
+        <v>2.7999722138947103</v>
       </c>
       <c r="W98" s="6">
-        <v>-1.9888027016935297</v>
+        <v>-4.334800042173066E-3</v>
       </c>
       <c r="X98" s="6">
-        <v>2.816080461680579</v>
+        <v>2.9855764779201559</v>
       </c>
       <c r="Y98" s="6">
-        <v>2.1053385732919381</v>
+        <v>1.8543778500428487</v>
       </c>
       <c r="Z98" s="6">
-        <v>0.22184218745858039</v>
+        <v>0.41437712885608741</v>
       </c>
       <c r="AA98" s="6">
-        <v>-3.1340571852849948</v>
+        <v>-2.6519795651680766</v>
       </c>
       <c r="AB98" s="6">
-        <v>-7.9767682441574186E-2</v>
+        <v>8.1967882980174836E-2</v>
       </c>
       <c r="AC98" s="6">
-        <v>2.3017376441058093</v>
+        <v>2.5326894631134462</v>
       </c>
       <c r="AD98" s="6">
-        <v>5.4334595959302776</v>
+        <v>5.0756568510671753</v>
       </c>
       <c r="AE98" s="6">
-        <v>6.8178921896044447</v>
+        <v>6.4064024621575291</v>
       </c>
       <c r="AF98" s="6">
-        <v>2.1045040145466829</v>
+        <v>2.6559036258003519</v>
       </c>
       <c r="AG98" s="6">
         <v>3.2279932806311606</v>
       </c>
       <c r="AH98" s="6">
-        <v>-0.73840743598546765</v>
+        <v>-0.59087405653857894</v>
       </c>
       <c r="AI98" s="6">
-        <v>1.2861993372248619</v>
+        <v>1.5170276511489749</v>
       </c>
       <c r="AJ98" s="6">
-        <v>1.0565022227382965</v>
+        <v>1.1924621450056274</v>
       </c>
       <c r="AK98" s="6">
-        <v>-0.85881494514051038</v>
+        <v>-0.17736380203700494</v>
       </c>
       <c r="AL98" s="6">
-        <v>2.0317157964513699</v>
+        <v>2.5440748920622096</v>
       </c>
       <c r="AM98" s="6">
-        <v>-0.45446964624819425</v>
+        <v>-1.2932586777004671</v>
       </c>
       <c r="AN98" s="6">
-        <v>2.8774411391027224</v>
+        <v>2.7497568290862908</v>
       </c>
       <c r="AO98" s="6">
-        <v>2.9520141269512621</v>
+        <v>2.9095014233026415</v>
       </c>
       <c r="AP98" s="6">
-        <v>1.0850017052316148</v>
+        <v>0.70025673522697107</v>
       </c>
       <c r="AQ98" s="6">
-        <v>1.6204911808284255</v>
+        <v>1.7281385442674255</v>
       </c>
       <c r="AR98" s="6">
-        <v>3.632421308771363</v>
+        <v>3.5340516634853874</v>
       </c>
       <c r="AS98" s="6">
-        <v>0.61798020359695582</v>
+        <v>0.90683564915752368</v>
       </c>
       <c r="AT98" s="6">
-        <v>-0.95515760656396165</v>
+        <v>-0.38870022789273728</v>
       </c>
       <c r="AU98" s="6">
-        <v>0.88266148967214197</v>
+        <v>1.0454474201444657</v>
       </c>
       <c r="AV98" s="6">
         <v>2.3737022812335042</v>
       </c>
       <c r="AW98" s="6">
-        <v>4.6753516593586797</v>
+        <v>4.6355056937479464</v>
       </c>
       <c r="AX98" s="6">
-        <v>3.4481268731281314</v>
+        <v>4.30470046454833</v>
       </c>
       <c r="AY98" s="6">
-        <v>-0.51768478998991851</v>
+        <v>-0.66096357107067227</v>
       </c>
       <c r="AZ98" s="6">
-        <v>-0.61760522440955579</v>
+        <v>-0.27867177946022642</v>
       </c>
       <c r="BA98" s="6">
-        <v>-2.558554764725379</v>
+        <v>-3.4194571934963092</v>
       </c>
     </row>
     <row r="99" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A99" s="5"/>
-      <c r="B99" s="6"/>
+      <c r="A99" s="5">
+        <v>42278</v>
+      </c>
+      <c r="B99" s="6">
+        <v>2.0109720293641753</v>
+      </c>
+      <c r="C99" s="6">
+        <v>3.875389073312093</v>
+      </c>
+      <c r="D99" s="6">
+        <v>1.6713264370977241</v>
+      </c>
+      <c r="E99" s="6">
+        <v>3.4988375535301701</v>
+      </c>
+      <c r="F99" s="6">
+        <v>0.43302394287164692</v>
+      </c>
+      <c r="G99" s="6">
+        <v>2.0792631730655082</v>
+      </c>
+      <c r="H99" s="6">
+        <v>1.2589464957269563</v>
+      </c>
+      <c r="I99" s="6">
+        <v>3.5758594401086343</v>
+      </c>
+      <c r="J99" s="6">
+        <v>6.3838400348970579</v>
+      </c>
+      <c r="K99" s="6">
+        <v>-8.3058752488200565</v>
+      </c>
+      <c r="L99" s="6">
+        <v>2.6486635728379273</v>
+      </c>
+      <c r="M99" s="6">
+        <v>1.6996638775173722</v>
+      </c>
+      <c r="N99" s="6">
+        <v>-1.4022928484078947</v>
+      </c>
+      <c r="O99" s="6">
+        <v>1.7020244649269953</v>
+      </c>
+      <c r="P99" s="6">
+        <v>1.6524800621482143</v>
+      </c>
+      <c r="Q99" s="6">
+        <v>1.0015035399525174</v>
+      </c>
+      <c r="R99" s="6">
+        <v>4.1900086022102334</v>
+      </c>
+      <c r="S99" s="6">
+        <v>0.70079406355546436</v>
+      </c>
+      <c r="T99" s="6">
+        <v>4.4161672817386926</v>
+      </c>
+      <c r="U99" s="6">
+        <v>-0.65807158333573323</v>
+      </c>
+      <c r="V99" s="6">
+        <v>3.1233671692587106</v>
+      </c>
+      <c r="W99" s="6">
+        <v>1.559358402569391</v>
+      </c>
+      <c r="X99" s="6">
+        <v>3.7401779270501736</v>
+      </c>
+      <c r="Y99" s="6">
+        <v>2.7034601909267413</v>
+      </c>
+      <c r="Z99" s="6">
+        <v>2.4437636772824591</v>
+      </c>
+      <c r="AA99" s="6">
+        <v>-0.95244836323532156</v>
+      </c>
+      <c r="AB99" s="6">
+        <v>-0.44515591527256249</v>
+      </c>
+      <c r="AC99" s="6">
+        <v>1.485635963187746</v>
+      </c>
+      <c r="AD99" s="6">
+        <v>6.0250952034602738</v>
+      </c>
+      <c r="AE99" s="6">
+        <v>5.8004642924436753</v>
+      </c>
+      <c r="AF99" s="6">
+        <v>4.202902598420188</v>
+      </c>
+      <c r="AG99" s="6">
+        <v>3.161060117917744</v>
+      </c>
+      <c r="AH99" s="6">
+        <v>-1.8565824674211004</v>
+      </c>
+      <c r="AI99" s="6">
+        <v>2.077786971076335</v>
+      </c>
+      <c r="AJ99" s="6">
+        <v>3.1326224220425574</v>
+      </c>
+      <c r="AK99" s="6">
+        <v>0.37679809409480747</v>
+      </c>
+      <c r="AL99" s="6">
+        <v>2.5351355087312619</v>
+      </c>
+      <c r="AM99" s="6">
+        <v>-0.71203965732984431</v>
+      </c>
+      <c r="AN99" s="6">
+        <v>3.3543683199632057</v>
+      </c>
+      <c r="AO99" s="6">
+        <v>3.6929845617981316</v>
+      </c>
+      <c r="AP99" s="6">
+        <v>-0.2734690259049502</v>
+      </c>
+      <c r="AQ99" s="6">
+        <v>2.2594997596382607</v>
+      </c>
+      <c r="AR99" s="6">
+        <v>4.6245140590792895</v>
+      </c>
+      <c r="AS99" s="6">
+        <v>2.1989038850612483</v>
+      </c>
+      <c r="AT99" s="6">
+        <v>-0.31218107179246302</v>
+      </c>
+      <c r="AU99" s="6">
+        <v>1.044125285500326</v>
+      </c>
+      <c r="AV99" s="6">
+        <v>3.0328898921944356</v>
+      </c>
+      <c r="AW99" s="6">
+        <v>3.4764430084489697</v>
+      </c>
+      <c r="AX99" s="6">
+        <v>5.6330882589008358</v>
+      </c>
+      <c r="AY99" s="6">
+        <v>0.4140175531080646</v>
+      </c>
+      <c r="AZ99" s="6">
+        <v>0.99756798909318467</v>
+      </c>
+      <c r="BA99" s="6">
+        <v>-2.8344035384745156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>